<commit_message>
more deploytimes! Moregit add .
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes .xlsx
+++ b/R/deploytimes/deploytimes .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22640" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>total</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>gemiddelde total</t>
-  </si>
-  <si>
     <t>puppet</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>gemiddelde config</t>
-  </si>
-  <si>
-    <t>variatie total</t>
   </si>
   <si>
     <t>10</t>
@@ -166,15 +160,55 @@
     <t>Kolom1</t>
   </si>
   <si>
-    <t>192</t>
+    <t>gemiddelde connection / pre</t>
+  </si>
+  <si>
+    <t>standard deviation config</t>
+  </si>
+  <si>
+    <t>Standard deviation config/pre</t>
+  </si>
+  <si>
+    <t>correllation between config</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -238,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -248,11 +282,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -527,11 +601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1778565264"/>
-        <c:axId val="-1778558000"/>
+        <c:axId val="-1920731392"/>
+        <c:axId val="-1920729072"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1778565264"/>
+        <c:axId val="-1920731392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +647,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1778558000"/>
+        <c:crossAx val="-1920729072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -581,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1778558000"/>
+        <c:axId val="-1920729072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +705,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1778565264"/>
+        <c:crossAx val="-1920731392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -916,11 +990,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1778528160"/>
-        <c:axId val="-1778526112"/>
+        <c:axId val="-1920707152"/>
+        <c:axId val="-1920704272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1778528160"/>
+        <c:axId val="-1920707152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +1036,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1778526112"/>
+        <c:crossAx val="-1920704272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -970,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1778526112"/>
+        <c:axId val="-1920704272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30.0"/>
@@ -1021,7 +1095,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1778528160"/>
+        <c:crossAx val="-1920707152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1117,6 +1191,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Deploytimes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1158,7 +1257,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Ansible!$A$7</c:f>
+              <c:f>Ansible!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1178,10 +1277,10 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Ansible!$B$7:$U$7</c:f>
+              <c:f>Ansible!$B$6:$AE$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>9.0</c:v>
                 </c:pt>
@@ -1241,6 +1340,36 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,7 +1380,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Ansible!$A$8</c:f>
+              <c:f>Ansible!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1271,10 +1400,10 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Ansible!$B$8:$U$8</c:f>
+              <c:f>Ansible!$B$7:$AE$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>67.0</c:v>
                 </c:pt>
@@ -1334,6 +1463,36 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>61.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,11 +1506,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1744262384"/>
-        <c:axId val="-1744259632"/>
+        <c:axId val="-1920668528"/>
+        <c:axId val="-1920665776"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1744262384"/>
+        <c:axId val="-1920668528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1393,7 +1552,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1744259632"/>
+        <c:crossAx val="-1920665776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1401,7 +1560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1744259632"/>
+        <c:axId val="-1920665776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1610,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1744262384"/>
+        <c:crossAx val="-1920668528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,8 +1726,14 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nl-NL"/>
-              <a:t>total</a:t>
+              <a:t>connection establishment</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1640,36 +1805,69 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Puppet!$B$4:$J$4</c:f>
+              <c:f>Puppet!$B$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>60.3</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.05</c:v>
+                  <c:v>5.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.36</c:v>
+                  <c:v>11.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.24</c:v>
+                  <c:v>6.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.74</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.61</c:v>
+                  <c:v>7.71</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.36</c:v>
+                  <c:v>6.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.0</c:v>
+                  <c:v>8.58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.57</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.76</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.56</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1706,59 +1904,91 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdDev"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Ansible!$B$2:$Q$2</c:f>
+              <c:f>Ansible!$B$6:$U$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>76.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>65.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>101.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>73.0</c:v>
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1775,11 +2005,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1740194304"/>
-        <c:axId val="-1716284720"/>
+        <c:axId val="-1920633408"/>
+        <c:axId val="-1920630928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1740194304"/>
+        <c:axId val="-1920633408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +2051,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1716284720"/>
+        <c:crossAx val="-1920630928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1829,7 +2059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1716284720"/>
+        <c:axId val="-1920630928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,7 +2140,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1740194304"/>
+        <c:crossAx val="-1920633408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2068,6 +2298,95 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ansible (deploy)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ansible!$B$7:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
@@ -2087,10 +2406,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Puppet!$B$5:$J$5</c:f>
+              <c:f>Puppet!$B$5:$U$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>51.35</c:v>
                 </c:pt>
@@ -2118,82 +2437,38 @@
                 <c:pt idx="8">
                   <c:v>43.29</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Ansible (deploy)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Ansible!$B$8:$Q$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45.0</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.0</c:v>
+                  <c:v>42.28</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52.0</c:v>
+                  <c:v>42.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53.0</c:v>
+                  <c:v>96.83</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54.0</c:v>
+                  <c:v>32.33</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52.0</c:v>
+                  <c:v>49.99</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>62.0</c:v>
+                  <c:v>40.32</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68.0</c:v>
+                  <c:v>55.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52.82</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2209,11 +2484,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1717634720"/>
-        <c:axId val="-1738153424"/>
+        <c:axId val="-1882908080"/>
+        <c:axId val="-1920604512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1717634720"/>
+        <c:axId val="-1882908080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2530,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1738153424"/>
+        <c:crossAx val="-1920604512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2263,7 +2538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1738153424"/>
+        <c:axId val="-1920604512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2619,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1717634720"/>
+        <c:crossAx val="-1882908080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5268,13 +5543,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>831850</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5303,13 +5578,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5332,15 +5607,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5363,39 +5638,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U5" totalsRowShown="0">
-  <autoFilter ref="A1:U5"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:AE5" totalsRowShown="0">
+  <autoFilter ref="A1:AE5"/>
+  <tableColumns count="31">
     <tableColumn id="1" name="in seconden"/>
-    <tableColumn id="2" name="1" dataDxfId="19"/>
-    <tableColumn id="3" name="2" dataDxfId="18"/>
-    <tableColumn id="4" name="3" dataDxfId="17"/>
-    <tableColumn id="5" name="4" dataDxfId="16"/>
-    <tableColumn id="6" name="5" dataDxfId="15"/>
-    <tableColumn id="7" name="6" dataDxfId="14"/>
-    <tableColumn id="8" name="7" dataDxfId="13"/>
-    <tableColumn id="9" name="8" dataDxfId="12"/>
-    <tableColumn id="10" name="9" dataDxfId="11"/>
-    <tableColumn id="11" name="10" dataDxfId="10"/>
-    <tableColumn id="12" name="11" dataDxfId="9"/>
-    <tableColumn id="13" name="12" dataDxfId="8"/>
-    <tableColumn id="14" name="13" dataDxfId="7"/>
-    <tableColumn id="15" name="14" dataDxfId="6"/>
-    <tableColumn id="16" name="15" dataDxfId="5"/>
-    <tableColumn id="17" name="16" dataDxfId="4"/>
-    <tableColumn id="18" name="17" dataDxfId="3"/>
-    <tableColumn id="19" name="18" dataDxfId="2"/>
-    <tableColumn id="20" name="19" dataDxfId="1"/>
-    <tableColumn id="21" name="20" dataDxfId="0"/>
+    <tableColumn id="2" name="1" dataDxfId="30"/>
+    <tableColumn id="3" name="2" dataDxfId="29"/>
+    <tableColumn id="4" name="3" dataDxfId="28"/>
+    <tableColumn id="5" name="4" dataDxfId="27"/>
+    <tableColumn id="6" name="5" dataDxfId="26"/>
+    <tableColumn id="7" name="6" dataDxfId="25"/>
+    <tableColumn id="8" name="7" dataDxfId="24"/>
+    <tableColumn id="9" name="8" dataDxfId="23"/>
+    <tableColumn id="10" name="9" dataDxfId="22"/>
+    <tableColumn id="11" name="10" dataDxfId="21"/>
+    <tableColumn id="12" name="11" dataDxfId="20"/>
+    <tableColumn id="13" name="12" dataDxfId="19"/>
+    <tableColumn id="14" name="13" dataDxfId="18"/>
+    <tableColumn id="15" name="14" dataDxfId="17"/>
+    <tableColumn id="16" name="15" dataDxfId="16"/>
+    <tableColumn id="17" name="16" dataDxfId="15"/>
+    <tableColumn id="18" name="17" dataDxfId="14"/>
+    <tableColumn id="19" name="18" dataDxfId="13"/>
+    <tableColumn id="20" name="19" dataDxfId="12"/>
+    <tableColumn id="21" name="20" dataDxfId="11"/>
+    <tableColumn id="22" name="21" dataDxfId="9"/>
+    <tableColumn id="23" name="22" dataDxfId="8"/>
+    <tableColumn id="24" name="23" dataDxfId="7"/>
+    <tableColumn id="25" name="24" dataDxfId="6"/>
+    <tableColumn id="26" name="25" dataDxfId="5"/>
+    <tableColumn id="27" name="26" dataDxfId="4"/>
+    <tableColumn id="28" name="27" dataDxfId="3"/>
+    <tableColumn id="29" name="28" dataDxfId="2"/>
+    <tableColumn id="30" name="29" dataDxfId="1"/>
+    <tableColumn id="31" name="30" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:U4" totalsRowShown="0">
-  <autoFilter ref="A1:U4"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:AE3" totalsRowShown="0">
+  <autoFilter ref="A1:AE3"/>
+  <tableColumns count="31">
     <tableColumn id="1" name="Kolom1"/>
     <tableColumn id="2" name="1"/>
     <tableColumn id="3" name="2"/>
@@ -5416,7 +5701,17 @@
     <tableColumn id="18" name="17"/>
     <tableColumn id="19" name="18"/>
     <tableColumn id="20" name="19"/>
-    <tableColumn id="21" name="192"/>
+    <tableColumn id="21" name="20"/>
+    <tableColumn id="22" name="21" dataDxfId="10"/>
+    <tableColumn id="23" name="22"/>
+    <tableColumn id="24" name="23"/>
+    <tableColumn id="25" name="24"/>
+    <tableColumn id="26" name="25"/>
+    <tableColumn id="27" name="26"/>
+    <tableColumn id="28" name="27"/>
+    <tableColumn id="29" name="28"/>
+    <tableColumn id="30" name="29"/>
+    <tableColumn id="31" name="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5685,10 +5980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5696,7 +5991,7 @@
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -5728,42 +6023,72 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>39</v>
+      <c r="V1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2">
         <v>8.9</v>
@@ -5825,10 +6150,28 @@
       <c r="U2" s="2">
         <v>7.41</v>
       </c>
+      <c r="V2" s="10">
+        <v>11</v>
+      </c>
+      <c r="W2" s="2">
+        <v>13</v>
+      </c>
+      <c r="X2" s="2">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2">
         <v>51.4</v>
@@ -5885,13 +6228,43 @@
         <v>72.73</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5967,18 +6340,46 @@
         <f t="shared" ref="S4" si="8">SUM(S2:S3)</f>
         <v>80.960000000000008</v>
       </c>
-      <c r="T4" s="2">
-        <f t="shared" ref="T4" si="9">SUM(T2:T3)</f>
-        <v>8</v>
-      </c>
-      <c r="U4" s="2">
-        <f t="shared" ref="U4" si="10">SUM(U2:U3)</f>
-        <v>7.41</v>
+      <c r="T4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2">
         <v>51.35</v>
@@ -6040,8 +6441,26 @@
       <c r="U5" s="2">
         <v>43.13</v>
       </c>
+      <c r="V5" s="10">
+        <v>47.43</v>
+      </c>
+      <c r="W5" s="2">
+        <v>56.98</v>
+      </c>
+      <c r="X5" s="2">
+        <v>59.97</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>61.28</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -6058,7 +6477,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6078,7 +6497,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6095,7 +6514,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6112,7 +6531,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6129,7 +6548,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6146,7 +6565,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -6163,7 +6582,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6180,7 +6599,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6197,7 +6616,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6214,7 +6633,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6317,10 +6736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6328,9 +6747,9 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -6360,40 +6779,70 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>45</v>
+      <c r="V1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -6457,8 +6906,38 @@
       <c r="U2">
         <v>50</v>
       </c>
+      <c r="V2" s="5">
+        <v>106</v>
+      </c>
+      <c r="W2">
+        <v>81</v>
+      </c>
+      <c r="X2">
+        <v>67</v>
+      </c>
+      <c r="Y2">
+        <v>67</v>
+      </c>
+      <c r="Z2">
+        <v>64</v>
+      </c>
+      <c r="AA2">
+        <v>69</v>
+      </c>
+      <c r="AB2">
+        <v>70</v>
+      </c>
+      <c r="AC2">
+        <v>71</v>
+      </c>
+      <c r="AD2">
+        <v>82</v>
+      </c>
+      <c r="AE2">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -6522,178 +7001,306 @@
       <c r="U3">
         <v>45</v>
       </c>
+      <c r="V3" s="5">
+        <v>96</v>
+      </c>
+      <c r="W3">
+        <v>73</v>
+      </c>
+      <c r="X3">
+        <v>61</v>
+      </c>
+      <c r="Y3">
+        <v>62</v>
+      </c>
+      <c r="Z3">
+        <v>59</v>
+      </c>
+      <c r="AA3">
+        <v>64</v>
+      </c>
+      <c r="AB3">
+        <v>65</v>
+      </c>
+      <c r="AC3">
+        <v>64</v>
+      </c>
+      <c r="AD3">
+        <v>76</v>
+      </c>
+      <c r="AE3">
+        <v>61</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6">
-        <f t="shared" ref="B7:I7" si="0">B2-B3</f>
+      <c r="B6" s="6">
+        <f t="shared" ref="B6:I6" si="0">B2-B3</f>
         <v>9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J7" s="6">
-        <f t="shared" ref="J7:N7" si="1">J2-J3</f>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6:N6" si="1">J2-J3</f>
         <v>4</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K6" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L6" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M6" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N6" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O7" s="6">
-        <f t="shared" ref="O7:T7" si="2">O2-O3</f>
+      <c r="O6" s="6">
+        <f t="shared" ref="O6:S6" si="2">O2-O3</f>
         <v>10</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P6" s="6">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q6" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R6" s="6">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S6" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="T7" s="6">
-        <f t="shared" ref="T7:U7" si="3">T2-T3</f>
+      <c r="T6" s="6">
+        <f t="shared" ref="T6:U6" si="3">T2-T3</f>
         <v>9</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U6" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
+      <c r="V6" s="5">
+        <f t="shared" ref="V6:Z6" si="4">V2-V3</f>
+        <v>10</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="Z6" s="6">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AA6" s="6">
+        <f t="shared" ref="AA6:AE6" si="5">AA2-AA3</f>
+        <v>5</v>
+      </c>
+      <c r="AB6" s="6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AC6" s="6">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AD6" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AE6" s="6">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6">
-        <f t="shared" ref="B8:I8" si="4">B3</f>
+      <c r="B7" s="6">
+        <f t="shared" ref="B7:I7" si="6">B3</f>
         <v>67</v>
       </c>
-      <c r="C8" s="6">
-        <f t="shared" si="4"/>
+      <c r="C7" s="6">
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="D8" s="6">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="4"/>
-        <v>59</v>
-      </c>
-      <c r="F8" s="6">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="4"/>
-        <v>59</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="4"/>
-        <v>57</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" ref="J8:N8" si="5">J3</f>
-        <v>45</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="5"/>
-        <v>90</v>
-      </c>
-      <c r="L8" s="6">
-        <f t="shared" si="5"/>
-        <v>52</v>
-      </c>
-      <c r="M8" s="6">
-        <f t="shared" si="5"/>
-        <v>53</v>
-      </c>
-      <c r="N8" s="6">
-        <f t="shared" si="5"/>
-        <v>54</v>
-      </c>
-      <c r="O8" s="6">
-        <f t="shared" ref="O8:T8" si="6">O3</f>
-        <v>52</v>
-      </c>
-      <c r="P8" s="6">
-        <f t="shared" si="6"/>
-        <v>62</v>
-      </c>
-      <c r="Q8" s="6">
-        <f t="shared" si="6"/>
-        <v>68</v>
-      </c>
-      <c r="R8" s="6">
+      <c r="D7" s="6">
         <f t="shared" si="6"/>
         <v>51</v>
       </c>
-      <c r="S8" s="6">
+      <c r="E7" s="6">
         <f t="shared" si="6"/>
         <v>59</v>
       </c>
-      <c r="T8" s="6">
-        <f t="shared" ref="T8:U8" si="7">T3</f>
+      <c r="F7" s="6">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="6"/>
+        <v>59</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="6"/>
+        <v>57</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:N7" si="7">J3</f>
+        <v>45</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="U8" s="6">
+      <c r="N7" s="6">
         <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" ref="O7:S7" si="8">O3</f>
+        <v>52</v>
+      </c>
+      <c r="P7" s="6">
+        <f t="shared" si="8"/>
+        <v>62</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="S7" s="6">
+        <f t="shared" si="8"/>
+        <v>59</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" ref="T7:U7" si="9">T3</f>
+        <v>53</v>
+      </c>
+      <c r="U7" s="6">
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
+      <c r="V7" s="5">
+        <f t="shared" ref="V7:Z7" si="10">V3</f>
+        <v>96</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="10"/>
+        <v>73</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="10"/>
+        <v>61</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="10"/>
+        <v>62</v>
+      </c>
+      <c r="Z7" s="6">
+        <f t="shared" si="10"/>
+        <v>59</v>
+      </c>
+      <c r="AA7" s="6">
+        <f t="shared" ref="AA7:AE7" si="11">AA3</f>
+        <v>64</v>
+      </c>
+      <c r="AB7" s="6">
+        <f t="shared" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="AC7" s="6">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="AD7" s="6">
+        <f t="shared" si="11"/>
+        <v>76</v>
+      </c>
+      <c r="AE7" s="6">
+        <f t="shared" si="11"/>
+        <v>61</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -6705,20 +7312,9 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -6728,10 +7324,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6747,52 +7343,68 @@
         <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2">
-        <f>AVERAGE(Puppet!B4:J4)</f>
-        <v>52.073333333333338</v>
-      </c>
-      <c r="D2">
-        <f>AVERAGE(Ansible!B2:Q2)</f>
-        <v>64.5</v>
+        <v>43</v>
+      </c>
+      <c r="C2" s="9">
+        <f>AVERAGE(Ansible!B6:U6)</f>
+        <v>6.25</v>
+      </c>
+      <c r="D2" s="9">
+        <f>AVERAGE(Tabel1[[#This Row],[1]:[20]])</f>
+        <v>7.5545</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="2">
-        <f>AVERAGE(Tabel1[[#This Row],[1]:[9]])</f>
-        <v>44.557777777777773</v>
-      </c>
-      <c r="D3" s="2">
-        <f>AVERAGE(Ansible!B8:Q8)</f>
-        <v>58.1875</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="9">
+        <f>STDEV(Ansible!B6:U6)</f>
+        <v>2.1244194253340942</v>
+      </c>
+      <c r="D3" s="9">
+        <f>STDEV(Puppet!B2:U2)</f>
+        <v>1.4570282481096533</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <f>VARPA(Tabel1[[#This Row],[1]:[9]])</f>
-        <v>58.693399999999613</v>
-      </c>
-      <c r="D4">
-        <f>VARPA(Ansible!B1:Q2)</f>
-        <v>1107.3125</v>
+        <v>26</v>
+      </c>
+      <c r="C4" s="9">
+        <f>AVERAGE(Ansible!B7:U7)</f>
+        <v>56.95</v>
+      </c>
+      <c r="D4" s="9">
+        <f>AVERAGE(Puppet!B5:U5)</f>
+        <v>47.063500000000012</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" t="e">
-        <f>st</f>
-        <v>#NAME?</v>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="9">
+        <f>STDEV(Ansible!B7:U7)</f>
+        <v>9.9444509784682307</v>
+      </c>
+      <c r="D5" s="9">
+        <f>STDEV(Puppet!B5:U5)</f>
+        <v>13.302964558797811</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <f>CORREL(Puppet!B5:U5,Ansible!B7:U7)</f>
+        <v>-4.5615856541784447E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>